<commit_message>
Finished data collection with graphs
</commit_message>
<xml_diff>
--- a/Lab_1/Data_Lab1.xlsx
+++ b/Lab_1/Data_Lab1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Measured vs Indicated" sheetId="5" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>Velocity (m/s)</t>
   </si>
@@ -157,14 +157,20 @@
   <si>
     <t>Thu Sep 12 10:49:55 2013</t>
   </si>
+  <si>
+    <t>LDA Velocity (m/s)</t>
+  </si>
+  <si>
+    <t>Timed Velocity (m/s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -287,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -304,9 +310,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -316,24 +319,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -343,20 +342,36 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,7 +431,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.6760025614196332E-2"/>
+          <c:x val="9.676002561419636E-2"/>
           <c:y val="3.433009876701041E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -523,9 +538,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'First Trial'!$H$17:$H$19</c:f>
+              <c:f>Timed!$F$19:$F$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.20312722222222221</c:v>
@@ -540,11 +555,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="106128896"/>
-        <c:axId val="106130432"/>
+        <c:axId val="65464960"/>
+        <c:axId val="91419008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106128896"/>
+        <c:axId val="65464960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,12 +594,12 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106130432"/>
+        <c:crossAx val="91419008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106130432"/>
+        <c:axId val="91419008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +628,7 @@
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106128896"/>
+        <c:crossAx val="65464960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -625,9 +640,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.59173407001828793"/>
-          <c:y val="3.5606307070410251E-2"/>
-          <c:w val="0.15705465346096142"/>
-          <c:h val="8.2651422131099314E-2"/>
+          <c:y val="3.5606307070410258E-2"/>
+          <c:w val="0.15705465346096145"/>
+          <c:h val="8.265142213109937E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -661,7 +676,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -994,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:T22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1011,12 +1026,12 @@
     <col min="11" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" s="11" customFormat="1">
-      <c r="B1" s="9"/>
-      <c r="C1" s="13" t="s">
+    <row r="1" spans="2:20" s="10" customFormat="1">
+      <c r="B1" s="8"/>
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1025,7 +1040,7 @@
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -1034,35 +1049,35 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="2:20">
       <c r="B2" s="6"/>
-      <c r="C2" s="8">
+      <c r="C2" s="22">
         <v>1</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="14">
         <v>3.6</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="15">
         <f>$D$16/D2</f>
         <v>0.24166666666666667</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="15">
         <f>E2*((0.05/D2)+(0.005/$D$16))</f>
         <v>4.7453703703703703E-3</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="26">
         <f>STDEV(E2:E4)</f>
         <v>6.7190106217982345E-3</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="23">
         <f>SUM(E2:E4)/3</f>
         <v>0.24179107679107678</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="19">
         <v>6.28</v>
       </c>
       <c r="K2" s="6"/>
@@ -1078,21 +1093,21 @@
     </row>
     <row r="3" spans="2:20">
       <c r="B3" s="6"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="24">
+      <c r="C3" s="22"/>
+      <c r="D3" s="14">
         <v>3.7</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="15">
         <f t="shared" ref="E3:E10" si="0">$D$16/D3</f>
         <v>0.23513513513513512</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="15">
         <f t="shared" ref="F3:F10" si="1">E3*((0.05/D3)+(0.005/$D$16))</f>
         <v>4.528853177501826E-3</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="21"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="20"/>
       <c r="K3" s="6"/>
       <c r="L3" s="4"/>
       <c r="M3" s="5"/>
@@ -1106,21 +1121,21 @@
     </row>
     <row r="4" spans="2:20">
       <c r="B4" s="6"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="24">
+      <c r="C4" s="22"/>
+      <c r="D4" s="14">
         <v>3.5</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="15">
         <f t="shared" si="0"/>
         <v>0.24857142857142858</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="15">
         <f t="shared" si="1"/>
         <v>4.9795918367346948E-3</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="22"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="21"/>
       <c r="K4" s="6"/>
       <c r="L4" s="4"/>
       <c r="M4" s="5"/>
@@ -1134,29 +1149,29 @@
     </row>
     <row r="5" spans="2:20">
       <c r="B5" s="6"/>
-      <c r="C5" s="8">
+      <c r="C5" s="22">
         <v>2</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="14">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="15">
         <f t="shared" si="0"/>
         <v>0.37826086956521743</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="15">
         <f t="shared" si="1"/>
         <v>1.0396975425330815E-2</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="26">
         <f>STDEV(E5:E7)</f>
         <v>1.6482463237002126E-2</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="23">
         <f t="shared" ref="H5" si="2">SUM(E5:E7)/3</f>
         <v>0.37873847167325431</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="19">
         <v>9.48</v>
       </c>
       <c r="K5" s="6"/>
@@ -1172,21 +1187,21 @@
     </row>
     <row r="6" spans="2:20">
       <c r="B6" s="6"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="24">
+      <c r="C6" s="22"/>
+      <c r="D6" s="14">
         <v>2.4</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="15">
         <f t="shared" si="0"/>
         <v>0.36249999999999999</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="15">
         <f t="shared" si="1"/>
         <v>9.6354166666666671E-3</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="21"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="20"/>
       <c r="K6" s="6"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -1200,21 +1215,21 @@
     </row>
     <row r="7" spans="2:20">
       <c r="B7" s="6"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="24">
+      <c r="C7" s="22"/>
+      <c r="D7" s="14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="15">
         <f t="shared" si="0"/>
         <v>0.39545454545454545</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="15">
         <f t="shared" si="1"/>
         <v>1.1260330578512397E-2</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="22"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="21"/>
       <c r="K7" s="6"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -1228,29 +1243,29 @@
     </row>
     <row r="8" spans="2:20">
       <c r="B8" s="6"/>
-      <c r="C8" s="8">
+      <c r="C8" s="22">
         <v>3</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="14">
         <v>1.8</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="15">
         <f t="shared" si="0"/>
         <v>0.48333333333333334</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="15">
         <f t="shared" si="1"/>
         <v>1.6203703703703706E-2</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="26">
         <f>STDEV(E8:E10)</f>
         <v>3.0225749496978729E-2</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="23">
         <f t="shared" ref="H8" si="3">SUM(E8:E10)/3</f>
         <v>0.51294934640522871</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>13.56</v>
       </c>
       <c r="K8" s="6"/>
@@ -1266,21 +1281,21 @@
     </row>
     <row r="9" spans="2:20">
       <c r="B9" s="6"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="24">
+      <c r="C9" s="22"/>
+      <c r="D9" s="14">
         <v>1.7</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="15">
         <f t="shared" si="0"/>
         <v>0.5117647058823529</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="15">
         <f t="shared" si="1"/>
         <v>1.7993079584775085E-2</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="21"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="20"/>
       <c r="K9" s="6"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -1294,21 +1309,21 @@
     </row>
     <row r="10" spans="2:20">
       <c r="B10" s="6"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="24">
+      <c r="C10" s="22"/>
+      <c r="D10" s="14">
         <v>1.6</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="15">
         <f t="shared" si="0"/>
         <v>0.54374999999999996</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="15">
         <f t="shared" si="1"/>
         <v>2.0117187499999998E-2</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="22"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="21"/>
       <c r="K10" s="6"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -1349,7 +1364,7 @@
       <c r="H12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="K12" s="6"/>
@@ -1370,10 +1385,10 @@
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="26">
+      <c r="H13" s="16">
         <v>1</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="17">
         <f>100*ABS(H2-I2)/H2</f>
         <v>2497.2836067173516</v>
       </c>
@@ -1395,10 +1410,10 @@
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="26">
+      <c r="H14" s="16">
         <v>2</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="17">
         <f>100*ABS(H5-I5)/H5</f>
         <v>2403.0464843240425</v>
       </c>
@@ -1414,10 +1429,10 @@
       <c r="T14" s="7"/>
     </row>
     <row r="15" spans="2:20">
-      <c r="H15" s="24">
+      <c r="H15" s="14">
         <v>3</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="17">
         <f>100*ABS(H8-I8)/H8</f>
         <v>2543.5358764036</v>
       </c>
@@ -1432,35 +1447,67 @@
       </c>
     </row>
     <row r="17" spans="4:8">
-      <c r="F17" s="28"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="4:8">
+      <c r="F18" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" spans="4:8">
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="29">
+        <f>AVERAGE('First Trial'!H7:H15)</f>
+        <v>0.20312722222222221</v>
+      </c>
+      <c r="G19" s="30">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="H19" s="31">
+        <v>6.28</v>
+      </c>
     </row>
     <row r="20" spans="4:8">
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="29">
+        <f>AVERAGE('Second Trial'!H7:H15)</f>
+        <v>0.31995022222222219</v>
+      </c>
+      <c r="G20" s="30">
+        <v>0.379</v>
+      </c>
+      <c r="H20" s="31">
+        <v>9.48</v>
+      </c>
     </row>
     <row r="21" spans="4:8">
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="29">
+        <f>AVERAGE('Third Trial'!H7:H15)</f>
+        <v>0.44163711111111115</v>
+      </c>
+      <c r="G21" s="30">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="H21" s="31">
+        <v>13.56</v>
+      </c>
     </row>
     <row r="22" spans="4:8">
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1484,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H17" sqref="H17:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1908,24 +1955,6 @@
       </c>
       <c r="L15">
         <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8">
-      <c r="H17">
-        <f>AVERAGE(H7:H15)</f>
-        <v>0.20312722222222221</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8">
-      <c r="H18">
-        <f>AVERAGE('Second Trial'!H7:H15)</f>
-        <v>0.31995022222222219</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8">
-      <c r="H19">
-        <f>AVERAGE('Third Trial'!H7:H15)</f>
-        <v>0.44163711111111115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>